<commit_message>
add resource(feilong-resources && feilong-common-test) maven model
</commit_message>
<xml_diff>
--- a/tools/feilong-office-excel/src/test/resources/loxia/excel/java集合框架报名.xlsx
+++ b/tools/feilong-office-excel/src/test/resources/loxia/excel/java集合框架报名.xlsx
@@ -8,16 +8,17 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="评价类型" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AH$1</definedName>
   </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="279">
   <si>
     <t>姓名</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -826,6 +827,206 @@
       </rPr>
       <t> </t>
     </r>
+  </si>
+  <si>
+    <t>P20140827</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>会议通知</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>培训时间安排</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>培训组织者态度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>培训教室布置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>现场次序维护</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表达清晰态度友善</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>对授课时间的掌控度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>现场气氛调节能力</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PPT内容</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PPT设计</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>对我有用</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>干货</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>是否满意老师</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>意见</t>
+  </si>
+  <si>
+    <t>意见</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>评价类型</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>评价内容</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>内容充实，但干货量少了点</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>沟通结果</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>希望了解Java集合框架设计思路，并且如何应用到实际的项目开发，这点会在以后的 设计模式专题中出现</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表扬</t>
+  </si>
+  <si>
+    <t>表扬</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>批评</t>
+  </si>
+  <si>
+    <t>批评</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>无</t>
+  </si>
+  <si>
+    <t>无</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>今天mp2项目发布!(非常大的感叹号) 建议周五。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nice</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.金总讲得好 2.金总讲得好 3.金总讲得好</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PPT不够完善</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PPT字体太小</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PPT字太小，看的吃力； 讲师比我帅！不能忍</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>讲得全，但举例不够全</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>建议多加代码例子</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>以前对java理论不是很足，也没有对源码过多的祥看，对这节课非常满意！</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>适当增加知识点的实例讲解</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.课堂的气氛很好 2.在课上学到很多 3.课程内容很有用</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>学到了一些实用的东西，希望公司以后能够提供职称考试</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>内容很丰富，讲得比较仔细，可以学到很多东西</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>① 专题明确 ②气氛比较好 ③有重点 ④希望更进一步的扩展</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.知识面涵盖了主要方面，2讲授比较好 3.下次希望可以在小部分内容深入一下</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>讲师很认真&lt;br/&gt;听课有效果</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>内容很丰富，讲师接地气 &lt;br/&gt;希望对涉及到的内容拓展一点</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.接地气，课程涉及较广，但具体细节较少 2 气氛融洽</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>通过本次课程的学习，对集合框架的认识有进一步的提升，金鑫老师对PPT的涉及很是用心。希望有更多类似的培训。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>干货，绝对的干货。提到的东西有一些遗忘的基本知识点，也有没用到的知识，有巩固到知识点也学习到了新的东西 赞</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>课件或PPT可先在课前给下否？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>very good &lt;br&gt;希望有对应知识点的一小段代码描述 &lt;br&gt;代码对程序员来说 来的比文字和语言来的更加直接.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>英语发音提高一点会更好，不然容易造成无解 very good</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>讲的很好！</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -870,12 +1071,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="微软雅黑"/>
-      <family val="2"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
       <name val="微软雅黑"/>
       <family val="2"/>
@@ -913,6 +1108,13 @@
       <name val="Verdana"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -940,7 +1142,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -952,7 +1154,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -961,31 +1163,40 @@
     <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1290,13 +1501,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J50"/>
+  <dimension ref="A1:AH50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B35" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="Q2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G52" sqref="G52"/>
+      <selection pane="bottomRight" activeCell="Z24" sqref="Z24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.15"/>
@@ -1309,12 +1520,29 @@
     <col min="6" max="6" width="13.875" style="4" customWidth="1"/>
     <col min="7" max="7" width="9.625" style="2" customWidth="1"/>
     <col min="8" max="8" width="11.625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="9.375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="23.125" style="4" customWidth="1"/>
-    <col min="11" max="16384" width="9" style="4"/>
+    <col min="9" max="9" width="7" style="2" customWidth="1"/>
+    <col min="10" max="10" width="12.875" style="4" customWidth="1"/>
+    <col min="11" max="11" width="10.875" style="2" customWidth="1"/>
+    <col min="12" max="12" width="8.125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="6.875" style="2" customWidth="1"/>
+    <col min="14" max="14" width="7.875" style="2" customWidth="1"/>
+    <col min="15" max="15" width="7.125" style="2" customWidth="1"/>
+    <col min="16" max="16" width="8.25" style="2" customWidth="1"/>
+    <col min="17" max="17" width="9.25" style="2" customWidth="1"/>
+    <col min="18" max="18" width="9.625" style="2" customWidth="1"/>
+    <col min="19" max="19" width="7.75" style="2" customWidth="1"/>
+    <col min="20" max="20" width="8.25" style="2" customWidth="1"/>
+    <col min="21" max="21" width="7.75" style="2" customWidth="1"/>
+    <col min="22" max="22" width="8.625" style="2" customWidth="1"/>
+    <col min="23" max="23" width="6.125" style="2" customWidth="1"/>
+    <col min="24" max="24" width="7.75" style="2" customWidth="1"/>
+    <col min="25" max="25" width="11.25" style="2" customWidth="1"/>
+    <col min="26" max="26" width="26.375" style="4" customWidth="1"/>
+    <col min="27" max="27" width="36.25" style="4" customWidth="1"/>
+    <col min="28" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:34" ht="48.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1345,277 +1573,743 @@
       <c r="J1" s="5" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="A2" s="12" t="s">
-        <v>26</v>
+      <c r="K1" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="L1" s="21" t="s">
+        <v>229</v>
+      </c>
+      <c r="M1" s="21" t="s">
+        <v>230</v>
+      </c>
+      <c r="N1" s="21" t="s">
+        <v>231</v>
+      </c>
+      <c r="O1" s="21" t="s">
+        <v>232</v>
+      </c>
+      <c r="P1" s="21" t="s">
+        <v>233</v>
+      </c>
+      <c r="Q1" s="21" t="s">
+        <v>234</v>
+      </c>
+      <c r="R1" s="21" t="s">
+        <v>235</v>
+      </c>
+      <c r="S1" s="21" t="s">
+        <v>236</v>
+      </c>
+      <c r="T1" s="21" t="s">
+        <v>237</v>
+      </c>
+      <c r="U1" s="21" t="s">
+        <v>238</v>
+      </c>
+      <c r="V1" s="21" t="s">
+        <v>239</v>
+      </c>
+      <c r="W1" s="21" t="s">
+        <v>240</v>
+      </c>
+      <c r="X1" s="21" t="s">
+        <v>241</v>
+      </c>
+      <c r="Y1" s="21" t="s">
+        <v>244</v>
+      </c>
+      <c r="Z1" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="AA1" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="AB1" s="5"/>
+      <c r="AC1" s="5"/>
+      <c r="AD1" s="5"/>
+      <c r="AE1" s="5"/>
+      <c r="AF1" s="5"/>
+      <c r="AG1" s="5"/>
+      <c r="AH1" s="5"/>
+    </row>
+    <row r="2" spans="1:34" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A2" s="17" t="s">
+        <v>81</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>82</v>
       </c>
       <c r="C2" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="G2" s="7">
+        <v>41878</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K2" s="2">
+        <v>1</v>
+      </c>
+      <c r="L2" s="2">
+        <v>5</v>
+      </c>
+      <c r="M2" s="2">
+        <v>4</v>
+      </c>
+      <c r="N2" s="2">
+        <v>5</v>
+      </c>
+      <c r="O2" s="2">
+        <v>5</v>
+      </c>
+      <c r="P2" s="2">
+        <v>5</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>5</v>
+      </c>
+      <c r="R2" s="2">
+        <v>5</v>
+      </c>
+      <c r="S2" s="2">
+        <v>5</v>
+      </c>
+      <c r="T2" s="2">
+        <v>5</v>
+      </c>
+      <c r="U2" s="2">
+        <v>5</v>
+      </c>
+      <c r="V2" s="2">
+        <v>4</v>
+      </c>
+      <c r="W2" s="2">
+        <v>3</v>
+      </c>
+      <c r="X2" s="2">
+        <v>3</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="Z2" s="4" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A3" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="G3" s="7">
+        <v>41878</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K3" s="2">
+        <v>1</v>
+      </c>
+      <c r="L3" s="2">
+        <v>5</v>
+      </c>
+      <c r="M3" s="2">
+        <v>4</v>
+      </c>
+      <c r="N3" s="2">
+        <v>5</v>
+      </c>
+      <c r="O3" s="2">
+        <v>5</v>
+      </c>
+      <c r="P3" s="2">
+        <v>5</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>5</v>
+      </c>
+      <c r="R3" s="2">
+        <v>4</v>
+      </c>
+      <c r="S3" s="2">
+        <v>5</v>
+      </c>
+      <c r="T3" s="2">
+        <v>5</v>
+      </c>
+      <c r="U3" s="2">
+        <v>5</v>
+      </c>
+      <c r="V3" s="2">
+        <v>4</v>
+      </c>
+      <c r="W3" s="2">
+        <v>3</v>
+      </c>
+      <c r="X3" s="2">
+        <v>3</v>
+      </c>
+      <c r="Y3" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="Z3" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="AA3" s="4" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A4" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="7">
+        <v>41878</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K4" s="2">
+        <v>1</v>
+      </c>
+      <c r="L4" s="2">
+        <v>5</v>
+      </c>
+      <c r="M4" s="2">
+        <v>4</v>
+      </c>
+      <c r="N4" s="2">
+        <v>5</v>
+      </c>
+      <c r="O4" s="2">
+        <v>4</v>
+      </c>
+      <c r="P4" s="2">
+        <v>5</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>5</v>
+      </c>
+      <c r="R4" s="2">
+        <v>4</v>
+      </c>
+      <c r="S4" s="2">
+        <v>5</v>
+      </c>
+      <c r="T4" s="2">
+        <v>5</v>
+      </c>
+      <c r="U4" s="2">
+        <v>5</v>
+      </c>
+      <c r="V4" s="2">
+        <v>4</v>
+      </c>
+      <c r="W4" s="2">
+        <v>3</v>
+      </c>
+      <c r="X4" s="2">
+        <v>3</v>
+      </c>
+      <c r="Y4" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="Z4" s="4" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A5" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="G5" s="7">
+        <v>41878</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K5" s="2">
+        <v>1</v>
+      </c>
+      <c r="L5" s="2">
+        <v>5</v>
+      </c>
+      <c r="M5" s="2">
+        <v>5</v>
+      </c>
+      <c r="N5" s="2">
+        <v>5</v>
+      </c>
+      <c r="O5" s="2">
+        <v>5</v>
+      </c>
+      <c r="P5" s="2">
+        <v>5</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>5</v>
+      </c>
+      <c r="R5" s="2">
+        <v>5</v>
+      </c>
+      <c r="S5" s="2">
+        <v>5</v>
+      </c>
+      <c r="T5" s="2">
+        <v>5</v>
+      </c>
+      <c r="U5" s="2">
+        <v>5</v>
+      </c>
+      <c r="V5" s="2">
+        <v>4</v>
+      </c>
+      <c r="W5" s="2">
+        <v>3</v>
+      </c>
+      <c r="X5" s="2">
+        <v>3</v>
+      </c>
+      <c r="Y5" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="Z5" s="4" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="6" spans="1:34" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A6" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="15" t="s">
-        <v>172</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>186</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="G2" s="7">
-        <v>41878</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="A3" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>170</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>186</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="G3" s="7">
-        <v>41878</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="A4" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>171</v>
-      </c>
-      <c r="E4" s="16" t="s">
-        <v>186</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" s="7">
-        <v>41878</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="A5" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>148</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="G5" s="7">
-        <v>41878</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I5" s="2">
+      <c r="D6" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="7">
+        <v>41878</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K6" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="A6" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>162</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="G6" s="7">
-        <v>41878</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I6" s="2">
+      <c r="L6" s="2">
+        <v>5</v>
+      </c>
+      <c r="M6" s="2">
+        <v>5</v>
+      </c>
+      <c r="N6" s="2">
+        <v>5</v>
+      </c>
+      <c r="O6" s="2">
+        <v>4</v>
+      </c>
+      <c r="P6" s="2">
+        <v>5</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>5</v>
+      </c>
+      <c r="R6" s="2">
+        <v>5</v>
+      </c>
+      <c r="S6" s="2">
+        <v>4</v>
+      </c>
+      <c r="T6" s="2">
+        <v>5</v>
+      </c>
+      <c r="U6" s="2">
+        <v>5</v>
+      </c>
+      <c r="V6" s="2">
+        <v>4</v>
+      </c>
+      <c r="X6" s="2">
+        <v>3</v>
+      </c>
+      <c r="Y6" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="Z6" s="4" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="7" spans="1:34" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A7" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G7" s="7">
+        <v>41878</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K7" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="A7" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>164</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="G7" s="7">
-        <v>41878</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I7" s="2">
+      <c r="L7" s="2">
+        <v>5</v>
+      </c>
+      <c r="M7" s="2">
+        <v>5</v>
+      </c>
+      <c r="N7" s="2">
+        <v>5</v>
+      </c>
+      <c r="O7" s="2">
+        <v>4</v>
+      </c>
+      <c r="P7" s="2">
+        <v>5</v>
+      </c>
+      <c r="Q7" s="2">
+        <v>5</v>
+      </c>
+      <c r="R7" s="2">
+        <v>5</v>
+      </c>
+      <c r="S7" s="2">
+        <v>5</v>
+      </c>
+      <c r="T7" s="2">
+        <v>5</v>
+      </c>
+      <c r="U7" s="2">
+        <v>5</v>
+      </c>
+      <c r="V7" s="2">
+        <v>4</v>
+      </c>
+      <c r="X7" s="2">
+        <v>3</v>
+      </c>
+      <c r="Y7" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="Z7" s="4" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="8" spans="1:34" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A8" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="7">
+        <v>41878</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K8" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="A8" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>163</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="G8" s="7">
-        <v>41878</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I8" s="2">
+      <c r="L8" s="2">
+        <v>5</v>
+      </c>
+      <c r="M8" s="2">
+        <v>5</v>
+      </c>
+      <c r="N8" s="2">
+        <v>5</v>
+      </c>
+      <c r="O8" s="2">
+        <v>5</v>
+      </c>
+      <c r="P8" s="2">
+        <v>5</v>
+      </c>
+      <c r="Q8" s="2">
+        <v>5</v>
+      </c>
+      <c r="R8" s="2">
+        <v>5</v>
+      </c>
+      <c r="S8" s="2">
+        <v>5</v>
+      </c>
+      <c r="T8" s="2">
+        <v>5</v>
+      </c>
+      <c r="U8" s="2">
+        <v>5</v>
+      </c>
+      <c r="V8" s="2">
+        <v>4</v>
+      </c>
+      <c r="W8" s="2">
+        <v>3</v>
+      </c>
+      <c r="X8" s="2">
+        <v>3</v>
+      </c>
+      <c r="Y8" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="Z8" s="4" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="9" spans="1:34" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A9" s="17" t="s">
+        <v>210</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>211</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="G9" s="7">
+        <v>41878</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K9" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="A9" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>165</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="G9" s="7">
-        <v>41878</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I9" s="2">
+      <c r="L9" s="2">
+        <v>5</v>
+      </c>
+      <c r="M9" s="2">
+        <v>5</v>
+      </c>
+      <c r="N9" s="2">
+        <v>5</v>
+      </c>
+      <c r="O9" s="2">
+        <v>5</v>
+      </c>
+      <c r="P9" s="2">
+        <v>5</v>
+      </c>
+      <c r="Q9" s="2">
+        <v>5</v>
+      </c>
+      <c r="R9" s="2">
+        <v>5</v>
+      </c>
+      <c r="S9" s="2">
+        <v>5</v>
+      </c>
+      <c r="T9" s="2">
+        <v>5</v>
+      </c>
+      <c r="U9" s="2">
+        <v>5</v>
+      </c>
+      <c r="V9" s="2">
+        <v>4</v>
+      </c>
+      <c r="W9" s="2">
+        <v>3</v>
+      </c>
+      <c r="X9" s="2">
+        <v>3</v>
+      </c>
+      <c r="Y9" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="Z9" s="4" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="10" spans="1:34" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A10" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="G10" s="7">
+        <v>41878</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K10" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="G10" s="7">
-        <v>41878</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I10" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11" s="11" t="s">
-        <v>9</v>
+      <c r="L10" s="2">
+        <v>5</v>
+      </c>
+      <c r="M10" s="2">
+        <v>5</v>
+      </c>
+      <c r="N10" s="2">
+        <v>5</v>
+      </c>
+      <c r="O10" s="2">
+        <v>5</v>
+      </c>
+      <c r="P10" s="2">
+        <v>5</v>
+      </c>
+      <c r="Q10" s="2">
+        <v>5</v>
+      </c>
+      <c r="R10" s="2">
+        <v>5</v>
+      </c>
+      <c r="S10" s="2">
+        <v>5</v>
+      </c>
+      <c r="T10" s="2">
+        <v>5</v>
+      </c>
+      <c r="U10" s="2">
+        <v>5</v>
+      </c>
+      <c r="V10" s="2">
+        <v>4</v>
+      </c>
+      <c r="W10" s="2">
+        <v>3</v>
+      </c>
+      <c r="X10" s="2">
+        <v>3</v>
+      </c>
+      <c r="Y10" s="2" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A11" s="17" t="s">
+        <v>101</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>158</v>
+        <v>103</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>168</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="F11" s="14" t="s">
-        <v>10</v>
+      <c r="F11" s="10" t="s">
+        <v>102</v>
       </c>
       <c r="G11" s="7">
         <v>41878</v>
@@ -1623,25 +2317,70 @@
       <c r="H11" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="A12" s="11" t="s">
-        <v>2</v>
+      <c r="K11" s="2">
+        <v>1</v>
+      </c>
+      <c r="L11" s="2">
+        <v>5</v>
+      </c>
+      <c r="M11" s="2">
+        <v>5</v>
+      </c>
+      <c r="N11" s="2">
+        <v>5</v>
+      </c>
+      <c r="O11" s="2">
+        <v>5</v>
+      </c>
+      <c r="P11" s="2">
+        <v>5</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>5</v>
+      </c>
+      <c r="R11" s="2">
+        <v>5</v>
+      </c>
+      <c r="S11" s="2">
+        <v>5</v>
+      </c>
+      <c r="T11" s="2">
+        <v>5</v>
+      </c>
+      <c r="U11" s="2">
+        <v>5</v>
+      </c>
+      <c r="V11" s="2">
+        <v>4</v>
+      </c>
+      <c r="W11" s="2">
+        <v>3</v>
+      </c>
+      <c r="X11" s="2">
+        <v>3</v>
+      </c>
+      <c r="Y11" s="2" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A12" s="17" t="s">
+        <v>64</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>160</v>
+        <v>65</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>169</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>127</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>132</v>
+        <v>66</v>
       </c>
       <c r="G12" s="7">
         <v>41878</v>
@@ -1649,25 +2388,70 @@
       <c r="H12" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A13" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>156</v>
+      <c r="K12" s="2">
+        <v>1</v>
+      </c>
+      <c r="L12" s="2">
+        <v>5</v>
+      </c>
+      <c r="M12" s="2">
+        <v>5</v>
+      </c>
+      <c r="N12" s="2">
+        <v>5</v>
+      </c>
+      <c r="O12" s="2">
+        <v>5</v>
+      </c>
+      <c r="P12" s="2">
+        <v>5</v>
+      </c>
+      <c r="Q12" s="2">
+        <v>5</v>
+      </c>
+      <c r="R12" s="2">
+        <v>5</v>
+      </c>
+      <c r="S12" s="2">
+        <v>5</v>
+      </c>
+      <c r="T12" s="2">
+        <v>5</v>
+      </c>
+      <c r="U12" s="2">
+        <v>5</v>
+      </c>
+      <c r="V12" s="2">
+        <v>4</v>
+      </c>
+      <c r="W12" s="2">
+        <v>3</v>
+      </c>
+      <c r="X12" s="2">
+        <v>3</v>
+      </c>
+      <c r="Y12" s="2" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="13" spans="1:34" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A13" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>218</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="F13" s="14" t="s">
-        <v>13</v>
+      <c r="F13" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="G13" s="7">
         <v>41878</v>
@@ -1675,25 +2459,73 @@
       <c r="H13" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="A14" s="12" t="s">
-        <v>19</v>
+      <c r="K13" s="2">
+        <v>1</v>
+      </c>
+      <c r="L13" s="2">
+        <v>5</v>
+      </c>
+      <c r="M13" s="2">
+        <v>5</v>
+      </c>
+      <c r="N13" s="2">
+        <v>5</v>
+      </c>
+      <c r="O13" s="2">
+        <v>5</v>
+      </c>
+      <c r="P13" s="2">
+        <v>5</v>
+      </c>
+      <c r="Q13" s="2">
+        <v>5</v>
+      </c>
+      <c r="R13" s="2">
+        <v>5</v>
+      </c>
+      <c r="S13" s="2">
+        <v>5</v>
+      </c>
+      <c r="T13" s="2">
+        <v>5</v>
+      </c>
+      <c r="U13" s="2">
+        <v>5</v>
+      </c>
+      <c r="V13" s="2">
+        <v>4</v>
+      </c>
+      <c r="W13" s="2">
+        <v>3</v>
+      </c>
+      <c r="X13" s="2">
+        <v>3</v>
+      </c>
+      <c r="Y13" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="Z13" s="4" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="14" spans="1:34" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A14" s="18" t="s">
+        <v>14</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="D14" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="12" t="s">
         <v>146</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="F14" s="4" t="s">
-        <v>126</v>
+      <c r="F14" s="11" t="s">
+        <v>10</v>
       </c>
       <c r="G14" s="7">
         <v>41878</v>
@@ -1701,51 +2533,148 @@
       <c r="H14" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A15" s="11" t="s">
-        <v>14</v>
+      <c r="K14" s="2">
+        <v>1</v>
+      </c>
+      <c r="L14" s="2">
+        <v>5</v>
+      </c>
+      <c r="M14" s="2">
+        <v>4</v>
+      </c>
+      <c r="N14" s="2">
+        <v>5</v>
+      </c>
+      <c r="O14" s="2">
+        <v>3</v>
+      </c>
+      <c r="P14" s="2">
+        <v>4</v>
+      </c>
+      <c r="Q14" s="2">
+        <v>4</v>
+      </c>
+      <c r="R14" s="2">
+        <v>4</v>
+      </c>
+      <c r="S14" s="2">
+        <v>5</v>
+      </c>
+      <c r="T14" s="2">
+        <v>5</v>
+      </c>
+      <c r="U14" s="2">
+        <v>4</v>
+      </c>
+      <c r="V14" s="2">
+        <v>4</v>
+      </c>
+      <c r="W14" s="2">
+        <v>3</v>
+      </c>
+      <c r="X14" s="2">
+        <v>3</v>
+      </c>
+      <c r="Y14" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="Z14" s="4" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="15" spans="1:34" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A15" s="17" t="s">
+        <v>89</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="G15" s="7">
+        <v>41878</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2">
+        <v>1</v>
+      </c>
+      <c r="L15" s="2">
+        <v>5</v>
+      </c>
+      <c r="M15" s="2">
+        <v>5</v>
+      </c>
+      <c r="N15" s="2">
+        <v>5</v>
+      </c>
+      <c r="O15" s="2">
+        <v>4</v>
+      </c>
+      <c r="P15" s="2">
+        <v>5</v>
+      </c>
+      <c r="Q15" s="2">
+        <v>5</v>
+      </c>
+      <c r="R15" s="2">
+        <v>5</v>
+      </c>
+      <c r="S15" s="2">
+        <v>5</v>
+      </c>
+      <c r="T15" s="2">
+        <v>5</v>
+      </c>
+      <c r="U15" s="2">
+        <v>5</v>
+      </c>
+      <c r="V15" s="2">
+        <v>4</v>
+      </c>
+      <c r="W15" s="2">
+        <v>3</v>
+      </c>
+      <c r="X15" s="2">
+        <v>3</v>
+      </c>
+      <c r="Y15" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="Z15" s="4" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="16" spans="1:34" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A16" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D16" s="12" t="s">
         <v>146</v>
       </c>
-      <c r="E15" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="F15" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="G15" s="7">
-        <v>41878</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="A16" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" s="15" t="s">
-        <v>175</v>
-      </c>
       <c r="E16" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="F16" s="14" t="s">
-        <v>132</v>
+        <v>136</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>92</v>
       </c>
       <c r="G16" s="7">
         <v>41878</v>
@@ -1753,155 +2682,443 @@
       <c r="H16" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="A17" s="12" t="s">
-        <v>22</v>
+      <c r="K16" s="2">
+        <v>1</v>
+      </c>
+      <c r="L16" s="2">
+        <v>5</v>
+      </c>
+      <c r="M16" s="2">
+        <v>5</v>
+      </c>
+      <c r="N16" s="2">
+        <v>5</v>
+      </c>
+      <c r="O16" s="2">
+        <v>4</v>
+      </c>
+      <c r="P16" s="2">
+        <v>5</v>
+      </c>
+      <c r="Q16" s="2">
+        <v>5</v>
+      </c>
+      <c r="R16" s="2">
+        <v>5</v>
+      </c>
+      <c r="S16" s="2">
+        <v>5</v>
+      </c>
+      <c r="T16" s="2">
+        <v>5</v>
+      </c>
+      <c r="U16" s="2">
+        <v>5</v>
+      </c>
+      <c r="V16" s="2">
+        <v>4</v>
+      </c>
+      <c r="W16" s="2">
+        <v>3</v>
+      </c>
+      <c r="X16" s="2">
+        <v>3</v>
+      </c>
+      <c r="Y16" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="Z16" s="4" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A17" s="17" t="s">
+        <v>76</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>23</v>
+        <v>77</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D17" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="G17" s="7">
+        <v>41878</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K17" s="2">
+        <v>1</v>
+      </c>
+      <c r="L17" s="2">
+        <v>5</v>
+      </c>
+      <c r="M17" s="2">
+        <v>5</v>
+      </c>
+      <c r="N17" s="2">
+        <v>5</v>
+      </c>
+      <c r="O17" s="2">
+        <v>4</v>
+      </c>
+      <c r="P17" s="2">
+        <v>5</v>
+      </c>
+      <c r="Q17" s="2">
+        <v>5</v>
+      </c>
+      <c r="R17" s="2">
+        <v>5</v>
+      </c>
+      <c r="S17" s="2">
+        <v>5</v>
+      </c>
+      <c r="T17" s="2">
+        <v>5</v>
+      </c>
+      <c r="U17" s="2">
+        <v>5</v>
+      </c>
+      <c r="V17" s="2">
+        <v>4</v>
+      </c>
+      <c r="W17" s="2">
+        <v>3</v>
+      </c>
+      <c r="X17" s="2">
+        <v>3</v>
+      </c>
+      <c r="Y17" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="Z17" s="4" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A18" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="G18" s="7">
+        <v>41878</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K18" s="2">
+        <v>1</v>
+      </c>
+      <c r="L18" s="2">
+        <v>5</v>
+      </c>
+      <c r="M18" s="2">
+        <v>5</v>
+      </c>
+      <c r="N18" s="2">
+        <v>5</v>
+      </c>
+      <c r="O18" s="2">
+        <v>5</v>
+      </c>
+      <c r="P18" s="2">
+        <v>5</v>
+      </c>
+      <c r="Q18" s="2">
+        <v>5</v>
+      </c>
+      <c r="R18" s="2">
+        <v>5</v>
+      </c>
+      <c r="S18" s="2">
+        <v>5</v>
+      </c>
+      <c r="T18" s="2">
+        <v>5</v>
+      </c>
+      <c r="U18" s="2">
+        <v>5</v>
+      </c>
+      <c r="V18" s="2">
+        <v>4</v>
+      </c>
+      <c r="W18" s="2">
+        <v>3</v>
+      </c>
+      <c r="X18" s="2">
+        <v>3</v>
+      </c>
+      <c r="Y18" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="Z18" s="4" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A19" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="D19" s="12" t="s">
         <v>146</v>
       </c>
-      <c r="E17" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="F17" s="10" t="s">
+      <c r="E19" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="G19" s="7">
+        <v>41878</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K19" s="2">
+        <v>1</v>
+      </c>
+      <c r="L19" s="2">
+        <v>5</v>
+      </c>
+      <c r="M19" s="2">
+        <v>5</v>
+      </c>
+      <c r="N19" s="2">
+        <v>5</v>
+      </c>
+      <c r="O19" s="2">
+        <v>5</v>
+      </c>
+      <c r="P19" s="2">
+        <v>5</v>
+      </c>
+      <c r="Q19" s="2">
+        <v>5</v>
+      </c>
+      <c r="R19" s="2">
+        <v>5</v>
+      </c>
+      <c r="S19" s="2">
+        <v>5</v>
+      </c>
+      <c r="T19" s="2">
+        <v>5</v>
+      </c>
+      <c r="U19" s="2">
+        <v>5</v>
+      </c>
+      <c r="V19" s="2">
+        <v>4</v>
+      </c>
+      <c r="W19" s="2">
+        <v>3</v>
+      </c>
+      <c r="X19" s="2">
+        <v>3</v>
+      </c>
+      <c r="Y19" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="Z19" s="4" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A20" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="G20" s="7">
+        <v>41878</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K20" s="2">
+        <v>1</v>
+      </c>
+      <c r="L20" s="2">
+        <v>5</v>
+      </c>
+      <c r="M20" s="2">
+        <v>5</v>
+      </c>
+      <c r="N20" s="2">
+        <v>5</v>
+      </c>
+      <c r="O20" s="2">
+        <v>5</v>
+      </c>
+      <c r="P20" s="2">
+        <v>5</v>
+      </c>
+      <c r="Q20" s="2">
+        <v>5</v>
+      </c>
+      <c r="R20" s="2">
+        <v>5</v>
+      </c>
+      <c r="S20" s="2">
+        <v>5</v>
+      </c>
+      <c r="T20" s="2">
+        <v>5</v>
+      </c>
+      <c r="U20" s="2">
+        <v>5</v>
+      </c>
+      <c r="V20" s="2">
+        <v>4</v>
+      </c>
+      <c r="W20" s="2">
+        <v>3</v>
+      </c>
+      <c r="X20" s="2">
+        <v>3</v>
+      </c>
+      <c r="Y20" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="Z20" s="4" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A21" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F21" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="G17" s="7">
-        <v>41878</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="A18" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="F18" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="G18" s="7">
-        <v>41878</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="A19" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19" s="15" t="s">
-        <v>168</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="F19" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="G19" s="7">
-        <v>41878</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="A20" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>167</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="F20" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="G20" s="7">
-        <v>41878</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="A21" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="D21" s="15" t="s">
-        <v>153</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="F21" s="10" t="s">
-        <v>69</v>
-      </c>
       <c r="G21" s="7">
         <v>41878</v>
       </c>
       <c r="H21" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="A22" s="12" t="s">
-        <v>62</v>
+      <c r="K21" s="2">
+        <v>1</v>
+      </c>
+      <c r="L21" s="2">
+        <v>5</v>
+      </c>
+      <c r="M21" s="2">
+        <v>5</v>
+      </c>
+      <c r="N21" s="2">
+        <v>5</v>
+      </c>
+      <c r="O21" s="2">
+        <v>4</v>
+      </c>
+      <c r="P21" s="2">
+        <v>5</v>
+      </c>
+      <c r="Q21" s="2">
+        <v>5</v>
+      </c>
+      <c r="R21" s="2">
+        <v>5</v>
+      </c>
+      <c r="S21" s="2">
+        <v>5</v>
+      </c>
+      <c r="T21" s="2">
+        <v>5</v>
+      </c>
+      <c r="U21" s="2">
+        <v>5</v>
+      </c>
+      <c r="V21" s="2">
+        <v>4</v>
+      </c>
+      <c r="W21" s="2">
+        <v>3</v>
+      </c>
+      <c r="X21" s="2">
+        <v>3</v>
+      </c>
+      <c r="Y21" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="Z21" s="4" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A22" s="18" t="s">
+        <v>9</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="D22" s="15" t="s">
-        <v>173</v>
+        <v>105</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>158</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="F22" s="10" t="s">
-        <v>132</v>
+      <c r="F22" s="11" t="s">
+        <v>10</v>
       </c>
       <c r="G22" s="7">
         <v>41878</v>
@@ -1909,25 +3126,73 @@
       <c r="H22" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="A23" s="12" t="s">
-        <v>64</v>
+      <c r="K22" s="2">
+        <v>1</v>
+      </c>
+      <c r="L22" s="2">
+        <v>5</v>
+      </c>
+      <c r="M22" s="2">
+        <v>5</v>
+      </c>
+      <c r="N22" s="2">
+        <v>5</v>
+      </c>
+      <c r="O22" s="2">
+        <v>4</v>
+      </c>
+      <c r="P22" s="2">
+        <v>5</v>
+      </c>
+      <c r="Q22" s="2">
+        <v>5</v>
+      </c>
+      <c r="R22" s="2">
+        <v>5</v>
+      </c>
+      <c r="S22" s="2">
+        <v>4</v>
+      </c>
+      <c r="T22" s="2">
+        <v>5</v>
+      </c>
+      <c r="U22" s="2">
+        <v>5</v>
+      </c>
+      <c r="V22" s="2">
+        <v>4</v>
+      </c>
+      <c r="W22" s="2">
+        <v>3</v>
+      </c>
+      <c r="X22" s="2">
+        <v>3</v>
+      </c>
+      <c r="Y22" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="Z22" s="4" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A23" s="18" t="s">
+        <v>12</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="D23" s="15" t="s">
-        <v>169</v>
+        <v>106</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>156</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="F23" s="10" t="s">
-        <v>66</v>
+      <c r="F23" s="11" t="s">
+        <v>13</v>
       </c>
       <c r="G23" s="7">
         <v>41878</v>
@@ -1935,25 +3200,73 @@
       <c r="H23" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="A24" s="12" t="s">
-        <v>55</v>
+      <c r="K23" s="2">
+        <v>1</v>
+      </c>
+      <c r="L23" s="2">
+        <v>5</v>
+      </c>
+      <c r="M23" s="2">
+        <v>5</v>
+      </c>
+      <c r="N23" s="2">
+        <v>5</v>
+      </c>
+      <c r="O23" s="2">
+        <v>4</v>
+      </c>
+      <c r="P23" s="2">
+        <v>5</v>
+      </c>
+      <c r="Q23" s="2">
+        <v>5</v>
+      </c>
+      <c r="R23" s="2">
+        <v>5</v>
+      </c>
+      <c r="S23" s="2">
+        <v>5</v>
+      </c>
+      <c r="T23" s="2">
+        <v>5</v>
+      </c>
+      <c r="U23" s="2">
+        <v>5</v>
+      </c>
+      <c r="V23" s="2">
+        <v>4</v>
+      </c>
+      <c r="W23" s="2">
+        <v>3</v>
+      </c>
+      <c r="X23" s="2">
+        <v>3</v>
+      </c>
+      <c r="Y23" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="Z23" s="4" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A24" s="17" t="s">
+        <v>18</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>57</v>
+        <v>108</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="D24" s="15" t="s">
-        <v>159</v>
+        <v>15</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>175</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="F24" s="10" t="s">
-        <v>56</v>
+      <c r="F24" s="11" t="s">
+        <v>132</v>
       </c>
       <c r="G24" s="7">
         <v>41878</v>
@@ -1961,25 +3274,73 @@
       <c r="H24" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="A25" s="12" t="s">
-        <v>47</v>
+      <c r="K24" s="2">
+        <v>1</v>
+      </c>
+      <c r="L24" s="2">
+        <v>5</v>
+      </c>
+      <c r="M24" s="2">
+        <v>5</v>
+      </c>
+      <c r="N24" s="2">
+        <v>5</v>
+      </c>
+      <c r="O24" s="2">
+        <v>5</v>
+      </c>
+      <c r="P24" s="2">
+        <v>5</v>
+      </c>
+      <c r="Q24" s="2">
+        <v>5</v>
+      </c>
+      <c r="R24" s="2">
+        <v>5</v>
+      </c>
+      <c r="S24" s="2">
+        <v>5</v>
+      </c>
+      <c r="T24" s="2">
+        <v>5</v>
+      </c>
+      <c r="U24" s="2">
+        <v>5</v>
+      </c>
+      <c r="V24" s="2">
+        <v>4</v>
+      </c>
+      <c r="W24" s="2">
+        <v>3</v>
+      </c>
+      <c r="X24" s="2">
+        <v>3</v>
+      </c>
+      <c r="Y24" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="Z24" s="4" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A25" s="17" t="s">
+        <v>68</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>49</v>
+        <v>67</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="D25" s="15" t="s">
-        <v>157</v>
+        <v>60</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>153</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>127</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
       <c r="G25" s="7">
         <v>41878</v>
@@ -1987,9 +3348,57 @@
       <c r="H25" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="A26" s="12" t="s">
+      <c r="K25" s="2">
+        <v>1</v>
+      </c>
+      <c r="L25" s="2">
+        <v>5</v>
+      </c>
+      <c r="M25" s="2">
+        <v>5</v>
+      </c>
+      <c r="N25" s="2">
+        <v>5</v>
+      </c>
+      <c r="O25" s="2">
+        <v>5</v>
+      </c>
+      <c r="P25" s="2">
+        <v>5</v>
+      </c>
+      <c r="Q25" s="2">
+        <v>5</v>
+      </c>
+      <c r="R25" s="2">
+        <v>5</v>
+      </c>
+      <c r="S25" s="2">
+        <v>5</v>
+      </c>
+      <c r="T25" s="2">
+        <v>4</v>
+      </c>
+      <c r="U25" s="2">
+        <v>4</v>
+      </c>
+      <c r="V25" s="2">
+        <v>4</v>
+      </c>
+      <c r="W25" s="2">
+        <v>3</v>
+      </c>
+      <c r="X25" s="2">
+        <v>3</v>
+      </c>
+      <c r="Y25" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="Z25" s="4" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A26" s="17" t="s">
         <v>37</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -1998,7 +3407,7 @@
       <c r="C26" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="D26" s="15" t="s">
+      <c r="D26" s="12" t="s">
         <v>166</v>
       </c>
       <c r="E26" s="3" t="s">
@@ -2016,9 +3425,57 @@
       <c r="J26" s="8" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="A27" s="12" t="s">
+      <c r="K26" s="2">
+        <v>1</v>
+      </c>
+      <c r="L26" s="2">
+        <v>5</v>
+      </c>
+      <c r="M26" s="2">
+        <v>5</v>
+      </c>
+      <c r="N26" s="2">
+        <v>5</v>
+      </c>
+      <c r="O26" s="2">
+        <v>5</v>
+      </c>
+      <c r="P26" s="2">
+        <v>5</v>
+      </c>
+      <c r="Q26" s="2">
+        <v>5</v>
+      </c>
+      <c r="R26" s="2">
+        <v>5</v>
+      </c>
+      <c r="S26" s="2">
+        <v>5</v>
+      </c>
+      <c r="T26" s="2">
+        <v>5</v>
+      </c>
+      <c r="U26" s="2">
+        <v>5</v>
+      </c>
+      <c r="V26" s="2">
+        <v>4</v>
+      </c>
+      <c r="W26" s="2">
+        <v>3</v>
+      </c>
+      <c r="X26" s="2">
+        <v>3</v>
+      </c>
+      <c r="Y26" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="Z26" s="4" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A27" s="17" t="s">
         <v>140</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -2027,7 +3484,7 @@
       <c r="C27" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="D27" s="15" t="s">
+      <c r="D27" s="12" t="s">
         <v>161</v>
       </c>
       <c r="E27" s="3" t="s">
@@ -2042,77 +3499,221 @@
       <c r="H27" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="A28" s="12" t="s">
+      <c r="K27" s="2">
+        <v>1</v>
+      </c>
+      <c r="L27" s="2">
+        <v>5</v>
+      </c>
+      <c r="M27" s="2">
+        <v>5</v>
+      </c>
+      <c r="N27" s="2">
+        <v>5</v>
+      </c>
+      <c r="O27" s="2">
+        <v>5</v>
+      </c>
+      <c r="P27" s="2">
+        <v>5</v>
+      </c>
+      <c r="Q27" s="2">
+        <v>5</v>
+      </c>
+      <c r="R27" s="2">
+        <v>5</v>
+      </c>
+      <c r="S27" s="2">
+        <v>4</v>
+      </c>
+      <c r="T27" s="2">
+        <v>5</v>
+      </c>
+      <c r="U27" s="2">
+        <v>5</v>
+      </c>
+      <c r="V27" s="2">
+        <v>4</v>
+      </c>
+      <c r="W27" s="2">
+        <v>3</v>
+      </c>
+      <c r="X27" s="2">
+        <v>3</v>
+      </c>
+      <c r="Y27" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="Z27" s="4" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A28" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="E28" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="G28" s="7">
+        <v>41878</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K28" s="2">
+        <v>1</v>
+      </c>
+      <c r="L28" s="2">
+        <v>5</v>
+      </c>
+      <c r="M28" s="2">
+        <v>5</v>
+      </c>
+      <c r="N28" s="2">
+        <v>5</v>
+      </c>
+      <c r="O28" s="2">
+        <v>5</v>
+      </c>
+      <c r="P28" s="2">
+        <v>5</v>
+      </c>
+      <c r="Q28" s="2">
+        <v>5</v>
+      </c>
+      <c r="R28" s="2">
+        <v>5</v>
+      </c>
+      <c r="S28" s="2">
+        <v>5</v>
+      </c>
+      <c r="T28" s="2">
+        <v>5</v>
+      </c>
+      <c r="U28" s="2">
+        <v>5</v>
+      </c>
+      <c r="V28" s="2">
+        <v>4</v>
+      </c>
+      <c r="W28" s="2">
+        <v>3</v>
+      </c>
+      <c r="X28" s="2">
+        <v>3</v>
+      </c>
+      <c r="Y28" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="Z28" s="4" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A29" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="E29" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="F29" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="G29" s="7">
+        <v>41878</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K29" s="2">
+        <v>1</v>
+      </c>
+      <c r="L29" s="2">
+        <v>5</v>
+      </c>
+      <c r="M29" s="2">
+        <v>5</v>
+      </c>
+      <c r="N29" s="2">
+        <v>5</v>
+      </c>
+      <c r="O29" s="2">
+        <v>5</v>
+      </c>
+      <c r="P29" s="2">
+        <v>5</v>
+      </c>
+      <c r="Q29" s="2">
+        <v>5</v>
+      </c>
+      <c r="R29" s="2">
+        <v>5</v>
+      </c>
+      <c r="S29" s="2">
+        <v>5</v>
+      </c>
+      <c r="T29" s="2">
+        <v>5</v>
+      </c>
+      <c r="U29" s="2">
+        <v>5</v>
+      </c>
+      <c r="V29" s="2">
+        <v>4</v>
+      </c>
+      <c r="W29" s="2">
+        <v>3</v>
+      </c>
+      <c r="X29" s="2">
+        <v>3</v>
+      </c>
+      <c r="Y29" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="Z29" s="4" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A30" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B30" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="C30" s="9" t="s">
         <v>199</v>
       </c>
-      <c r="D28" s="15" t="s">
+      <c r="D30" s="12" t="s">
         <v>204</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="F28" s="10" t="s">
-        <v>197</v>
-      </c>
-      <c r="G28" s="7">
-        <v>41878</v>
-      </c>
-      <c r="H28" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="A29" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>193</v>
-      </c>
-      <c r="D29" s="15" t="s">
-        <v>203</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="F29" s="10" t="s">
-        <v>195</v>
-      </c>
-      <c r="G29" s="7">
-        <v>41878</v>
-      </c>
-      <c r="H29" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="A30" s="12" t="s">
-        <v>188</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>190</v>
-      </c>
-      <c r="D30" s="15" t="s">
-        <v>191</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>127</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>32</v>
+        <v>197</v>
       </c>
       <c r="G30" s="7">
         <v>41878</v>
@@ -2120,25 +3721,31 @@
       <c r="H30" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="A31" s="12" t="s">
-        <v>223</v>
-      </c>
-      <c r="B31" s="17" t="s">
-        <v>205</v>
+      <c r="K30" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y30" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A31" s="17" t="s">
+        <v>192</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>194</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>206</v>
-      </c>
-      <c r="D31" s="15" t="s">
-        <v>218</v>
+        <v>193</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>203</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>127</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>32</v>
+        <v>195</v>
       </c>
       <c r="G31" s="7">
         <v>41878</v>
@@ -2146,25 +3753,31 @@
       <c r="H31" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="A32" s="12" t="s">
-        <v>207</v>
-      </c>
-      <c r="B32" s="17" t="s">
-        <v>208</v>
+      <c r="K31" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y31" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A32" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>209</v>
-      </c>
-      <c r="D32" s="15" t="s">
-        <v>219</v>
+        <v>15</v>
+      </c>
+      <c r="D32" s="12" t="s">
+        <v>144</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>10</v>
+        <v>92</v>
       </c>
       <c r="G32" s="7">
         <v>41878</v>
@@ -2172,25 +3785,28 @@
       <c r="H32" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="A33" s="12" t="s">
-        <v>210</v>
-      </c>
-      <c r="B33" s="17" t="s">
-        <v>211</v>
+      <c r="Y32" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="33" spans="1:25" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A33" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>212</v>
-      </c>
-      <c r="D33" s="15" t="s">
-        <v>220</v>
+        <v>45</v>
+      </c>
+      <c r="D33" s="12" t="s">
+        <v>155</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F33" s="10" t="s">
-        <v>213</v>
+        <v>25</v>
       </c>
       <c r="G33" s="7">
         <v>41878</v>
@@ -2198,25 +3814,28 @@
       <c r="H33" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="A34" s="12" t="s">
-        <v>93</v>
+      <c r="Y33" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="34" spans="1:25" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A34" s="17" t="s">
+        <v>178</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>95</v>
+        <v>179</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="D34" s="15" t="s">
-        <v>154</v>
+        <v>182</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>184</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>128</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>25</v>
+        <v>180</v>
       </c>
       <c r="G34" s="7">
         <v>41878</v>
@@ -2224,19 +3843,22 @@
       <c r="H34" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="A35" s="12" t="s">
-        <v>44</v>
+      <c r="Y34" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="35" spans="1:25" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A35" s="17" t="s">
+        <v>176</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>46</v>
+        <v>177</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="D35" s="15" t="s">
-        <v>155</v>
+        <v>181</v>
+      </c>
+      <c r="D35" s="12" t="s">
+        <v>183</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>128</v>
@@ -2250,51 +3872,55 @@
       <c r="H35" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="A36" s="12" t="s">
-        <v>120</v>
+      <c r="Y35" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A36" s="17" t="s">
+        <v>200</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>121</v>
+        <v>201</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="D36" s="15" t="s">
-        <v>152</v>
+        <v>202</v>
+      </c>
+      <c r="D36" s="12" t="s">
+        <v>217</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="F36" s="10" t="s">
-        <v>128</v>
-      </c>
+      <c r="F36" s="10"/>
       <c r="G36" s="7">
         <v>41878</v>
       </c>
       <c r="H36" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="A37" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="C37" s="9" t="s">
-        <v>182</v>
+      <c r="Y36" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A37" s="20" t="s">
+        <v>224</v>
+      </c>
+      <c r="B37" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>226</v>
       </c>
       <c r="D37" s="15" t="s">
-        <v>184</v>
+        <v>227</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>128</v>
       </c>
       <c r="F37" s="10" t="s">
-        <v>180</v>
+        <v>25</v>
       </c>
       <c r="G37" s="7">
         <v>41878</v>
@@ -2302,25 +3928,28 @@
       <c r="H37" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="A38" s="12" t="s">
-        <v>176</v>
+      <c r="Y37" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A38" s="17" t="s">
+        <v>19</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>177</v>
+        <v>20</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="D38" s="15" t="s">
-        <v>183</v>
+        <v>110</v>
+      </c>
+      <c r="D38" s="12" t="s">
+        <v>146</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="F38" s="10" t="s">
-        <v>25</v>
+        <v>127</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>126</v>
       </c>
       <c r="G38" s="7">
         <v>41878</v>
@@ -2328,49 +3957,59 @@
       <c r="H38" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="A39" s="12" t="s">
-        <v>200</v>
+      <c r="Y38" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="39" spans="1:25" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A39" s="17" t="s">
+        <v>31</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>201</v>
+        <v>33</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="D39" s="15" t="s">
-        <v>217</v>
+        <v>34</v>
+      </c>
+      <c r="D39" s="12" t="s">
+        <v>174</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="F39" s="10"/>
+        <v>127</v>
+      </c>
+      <c r="F39" s="10" t="s">
+        <v>32</v>
+      </c>
       <c r="G39" s="7">
         <v>41878</v>
       </c>
       <c r="H39" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="A40" s="12" t="s">
-        <v>214</v>
-      </c>
-      <c r="B40" s="17" t="s">
-        <v>215</v>
+      <c r="K39" s="16"/>
+      <c r="L39" s="16"/>
+      <c r="Y39" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="40" spans="1:25" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A40" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>86</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>216</v>
-      </c>
-      <c r="D40" s="15" t="s">
-        <v>221</v>
+        <v>87</v>
+      </c>
+      <c r="D40" s="12" t="s">
+        <v>167</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F40" s="10" t="s">
-        <v>25</v>
+        <v>88</v>
       </c>
       <c r="G40" s="7">
         <v>41878</v>
@@ -2378,25 +4017,28 @@
       <c r="H40" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="A41" s="12" t="s">
-        <v>42</v>
+      <c r="Y40" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="41" spans="1:25" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A41" s="17" t="s">
+        <v>62</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="D41" s="15" t="s">
-        <v>150</v>
+        <v>60</v>
+      </c>
+      <c r="D41" s="12" t="s">
+        <v>173</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="F41" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G41" s="7">
         <v>41878</v>
@@ -2404,25 +4046,28 @@
       <c r="H41" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="A42" s="12" t="s">
-        <v>138</v>
+      <c r="Y41" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="42" spans="1:25" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A42" s="17" t="s">
+        <v>47</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D42" s="15" t="s">
-        <v>151</v>
+        <v>50</v>
+      </c>
+      <c r="D42" s="12" t="s">
+        <v>157</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="F42" s="10" t="s">
-        <v>137</v>
+        <v>48</v>
       </c>
       <c r="G42" s="7">
         <v>41878</v>
@@ -2430,25 +4075,28 @@
       <c r="H42" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="A43" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>75</v>
+      <c r="Y42" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="43" spans="1:25" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A43" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="B43" s="14" t="s">
+        <v>208</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D43" s="15" t="s">
-        <v>144</v>
+        <v>209</v>
+      </c>
+      <c r="D43" s="12" t="s">
+        <v>219</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="F43" s="10" t="s">
-        <v>92</v>
+        <v>10</v>
       </c>
       <c r="G43" s="7">
         <v>41878</v>
@@ -2456,25 +4104,28 @@
       <c r="H43" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="A44" s="12" t="s">
-        <v>89</v>
+      <c r="Y43" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="44" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A44" s="18" t="s">
+        <v>83</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="D44" s="15" t="s">
-        <v>143</v>
+        <v>112</v>
+      </c>
+      <c r="D44" s="12" t="s">
+        <v>146</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="F44" s="10" t="s">
-        <v>92</v>
+        <v>125</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>124</v>
       </c>
       <c r="G44" s="7">
         <v>41878</v>
@@ -2482,22 +4133,28 @@
       <c r="H44" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="A45" s="12" t="s">
-        <v>81</v>
+      <c r="I44" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y44" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="45" spans="1:25" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A45" s="17" t="s">
+        <v>97</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="D45" s="15" t="s">
-        <v>145</v>
+        <v>87</v>
+      </c>
+      <c r="D45" s="12" t="s">
+        <v>164</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="F45" s="10" t="s">
         <v>92</v>
@@ -2508,25 +4165,31 @@
       <c r="H45" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="A46" s="12" t="s">
-        <v>70</v>
+      <c r="I45" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y45" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="46" spans="1:25" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A46" s="17" t="s">
+        <v>78</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D46" s="15" t="s">
-        <v>146</v>
+        <v>80</v>
+      </c>
+      <c r="D46" s="12" t="s">
+        <v>163</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="F46" s="10" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
       <c r="G46" s="7">
         <v>41878</v>
@@ -2534,25 +4197,31 @@
       <c r="H46" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="A47" s="12" t="s">
-        <v>76</v>
+      <c r="I46" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y46" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="47" spans="1:25" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A47" s="17" t="s">
+        <v>51</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>77</v>
+        <v>54</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D47" s="15" t="s">
-        <v>147</v>
+        <v>53</v>
+      </c>
+      <c r="D47" s="12" t="s">
+        <v>165</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="F47" s="10" t="s">
-        <v>92</v>
+        <v>52</v>
       </c>
       <c r="G47" s="7">
         <v>41878</v>
@@ -2560,22 +4229,28 @@
       <c r="H47" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="A48" s="12" t="s">
-        <v>117</v>
+      <c r="I47" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y47" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="48" spans="1:25" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A48" s="17" t="s">
+        <v>35</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>118</v>
+        <v>36</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="D48" s="15" t="s">
-        <v>149</v>
+        <v>113</v>
+      </c>
+      <c r="D48" s="12" t="s">
+        <v>148</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>136</v>
+        <v>222</v>
       </c>
       <c r="F48" s="10" t="s">
         <v>92</v>
@@ -2586,25 +4261,31 @@
       <c r="H48" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="A49" s="12" t="s">
-        <v>116</v>
+      <c r="I48" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y48" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="49" spans="1:25" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A49" s="19" t="s">
+        <v>16</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="D49" s="15" t="s">
-        <v>146</v>
+        <v>17</v>
+      </c>
+      <c r="D49" s="12" t="s">
+        <v>162</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="F49" s="10" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
       <c r="G49" s="7">
         <v>41878</v>
@@ -2612,25 +4293,31 @@
       <c r="H49" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A50" s="18" t="s">
-        <v>224</v>
-      </c>
-      <c r="B50" s="17" t="s">
-        <v>225</v>
-      </c>
-      <c r="C50" s="17" t="s">
-        <v>226</v>
-      </c>
-      <c r="D50" s="18" t="s">
-        <v>227</v>
-      </c>
-      <c r="E50" s="3" t="s">
-        <v>128</v>
+      <c r="I49" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y49" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="50" spans="1:25" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A50" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D50" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="E50" s="13" t="s">
+        <v>186</v>
       </c>
       <c r="F50" s="10" t="s">
-        <v>25</v>
+        <v>187</v>
       </c>
       <c r="G50" s="7">
         <v>41878</v>
@@ -2638,18 +4325,69 @@
       <c r="H50" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="Y50" s="2" t="s">
+        <v>249</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J1">
-    <sortState ref="A2:J49">
-      <sortCondition ref="E1"/>
+  <autoFilter ref="A1:AH1">
+    <sortState ref="A2:AH50">
+      <sortCondition descending="1" ref="Y1"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B14" r:id="rId1"/>
+    <hyperlink ref="B38" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>评价类型!$A$1:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>Y2:Y50</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>254</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>